<commit_message>
misc changes to wrappers, small changes to functions calling spm and fsl preprocessing
</commit_message>
<xml_diff>
--- a/dependencies/xlwrite-default-workbook.xlsx
+++ b/dependencies/xlwrite-default-workbook.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="6500" yWindow="4600" windowWidth="38360" windowHeight="21020" tabRatio="500"/>
+    <workbookView xWindow="20" yWindow="460" windowWidth="25580" windowHeight="28220" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Default" sheetId="1" r:id="rId1"/>
@@ -522,9 +522,9 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="55">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+  <cellStyleXfs count="57">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" applyBorder="0">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -572,36 +572,45 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="2" fontId="18" fillId="0" borderId="10">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="2" fontId="18" fillId="0" borderId="10" applyBorder="0">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="10">
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="10" applyBorder="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="33" borderId="10" applyBorder="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="34" borderId="10" applyBorder="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="10" applyBorder="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="18" fillId="0" borderId="10" applyBorder="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" applyNumberFormat="0" applyFont="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="21" fillId="33" borderId="10">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFont="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="21" fillId="34" borderId="10">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="10">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="18" fillId="0" borderId="10">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="50" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="55">
+  <cellStyles count="57">
     <cellStyle name="20% - Accent1" xfId="24" builtinId="30" hidden="1"/>
     <cellStyle name="20% - Accent2" xfId="28" builtinId="34" hidden="1"/>
     <cellStyle name="20% - Accent3" xfId="32" builtinId="38" hidden="1"/>
@@ -626,6 +635,7 @@
     <cellStyle name="Accent4" xfId="35" builtinId="41" hidden="1"/>
     <cellStyle name="Accent5" xfId="39" builtinId="45" hidden="1"/>
     <cellStyle name="Accent6" xfId="43" builtinId="49" hidden="1"/>
+    <cellStyle name="Add Border" xfId="55"/>
     <cellStyle name="Bad" xfId="12" builtinId="27" hidden="1"/>
     <cellStyle name="Calculation" xfId="16" builtinId="22" hidden="1"/>
     <cellStyle name="Check Cell" xfId="18" builtinId="23" hidden="1"/>
@@ -634,6 +644,7 @@
     <cellStyle name="Comma [0]" xfId="2" builtinId="6" hidden="1"/>
     <cellStyle name="Currency" xfId="3" builtinId="4" hidden="1"/>
     <cellStyle name="Currency [0]" xfId="4" builtinId="7" hidden="1"/>
+    <cellStyle name="Delete Border" xfId="56"/>
     <cellStyle name="Explanatory Text" xfId="21" builtinId="53" hidden="1"/>
     <cellStyle name="Float-2" xfId="47"/>
     <cellStyle name="Float-3" xfId="53"/>
@@ -934,19 +945,20 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <tabColor rgb="FF00B050"/>
   </sheetPr>
-  <dimension ref="A3"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="87" zoomScaleNormal="87" zoomScalePageLayoutView="87" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="87" zoomScaleNormal="87" zoomScalePageLayoutView="87" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.85546875" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="16384" width="9.85546875" style="1"/>
+    <col min="1" max="16384" width="9.85546875" style="2"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1"/>
+    </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
     </row>

</xml_diff>